<commit_message>
Update Puesta en Operación Gobierno Iván Duque.xlsx
</commit_message>
<xml_diff>
--- a/Infraestructura/Puesta en Operación Gobierno Iván Duque.xlsx
+++ b/Infraestructura/Puesta en Operación Gobierno Iván Duque.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmadrid/Documents/GitHub/Dotaciones2019/Infraestructura/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB81810-3B6B-F64B-A22F-D355F462B51A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C24271F-AE9F-2644-BD0D-ED12E3602783}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8420" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORTE CDI GOBIERNO DUQUE" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
   <si>
     <t>NOMBRE CDI</t>
   </si>
@@ -205,6 +205,15 @@
   </si>
   <si>
     <t>DONANTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALLE DEL CAUCA </t>
+  </si>
+  <si>
+    <t>YOTOCO</t>
+  </si>
+  <si>
+    <t>CDI SEMILLITAS</t>
   </si>
 </sst>
 </file>
@@ -715,7 +724,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -728,9 +737,9 @@
     <col min="6" max="6" width="50.5" style="2" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="11.5" style="2"/>
-    <col min="9" max="9" width="13.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="2"/>
-    <col min="11" max="11" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.33203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" style="2" customWidth="1"/>
     <col min="12" max="16384" width="11.5" style="2"/>
   </cols>
   <sheetData>
@@ -1088,11 +1097,21 @@
       <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="A15" s="14">
+        <v>13</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="4">
+        <v>43520</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>53</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="15"/>
@@ -1249,6 +1268,6 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="61" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="61" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>